<commit_message>
added aliquot plates for hiseq2
</commit_message>
<xml_diff>
--- a/DAB/aliquot_plates/NGS.Plates.Barcodes.DAB2017.Final.xlsx
+++ b/DAB/aliquot_plates/NGS.Plates.Barcodes.DAB2017.Final.xlsx
@@ -14,7 +14,6 @@
   <sheets>
     <sheet name="PCR_Plates_4Reps" sheetId="4" r:id="rId1"/>
     <sheet name="Ekstra-Tkiva" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="42">
   <si>
     <t>Aliquot Plate</t>
   </si>
@@ -76,16 +75,10 @@
     <t>AliquotPlate_BC</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>A45</t>
   </si>
   <si>
     <t>A46</t>
-  </si>
-  <si>
-    <t>PP???</t>
   </si>
   <si>
     <t>A47</t>
@@ -111,12 +104,60 @@
   <si>
     <t>A52</t>
   </si>
+  <si>
+    <t>DAB023_A45_PP1</t>
+  </si>
+  <si>
+    <t>DAB023_A45_PP8</t>
+  </si>
+  <si>
+    <t>DAB023_A46_PP2</t>
+  </si>
+  <si>
+    <t>DAB023_A46_PP7</t>
+  </si>
+  <si>
+    <t>DAB023_A47_PP3</t>
+  </si>
+  <si>
+    <t>DAB023_A47_PP6</t>
+  </si>
+  <si>
+    <t>DAB023_A48_PP4</t>
+  </si>
+  <si>
+    <t>DAB023_A48_PP5</t>
+  </si>
+  <si>
+    <t>DAB024_A49_PP1</t>
+  </si>
+  <si>
+    <t>DAB024_A49_PP8</t>
+  </si>
+  <si>
+    <t>DAB024_A50_PP2</t>
+  </si>
+  <si>
+    <t>DAB024_A50_PP7</t>
+  </si>
+  <si>
+    <t>DAB024_A51_PP3</t>
+  </si>
+  <si>
+    <t>DAB024_A51_PP6</t>
+  </si>
+  <si>
+    <t>DAB024_A52_PP4</t>
+  </si>
+  <si>
+    <t>DAB024_A52_PP5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,16 +190,8 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,11 +206,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -220,21 +248,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
+  <cellStyles count="3">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -517,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5095,7 +5120,7 @@
         <v>A35</v>
       </c>
       <c r="G139" s="2" t="str">
-        <f t="shared" ref="G139:G177" si="14">A139&amp;D139</f>
+        <f t="shared" ref="G139:G193" si="14">A139&amp;D139</f>
         <v>DAB18</v>
       </c>
       <c r="H139">
@@ -5968,7 +5993,7 @@
         <v>4</v>
       </c>
       <c r="B166" s="2" t="str">
-        <f t="shared" ref="B166:B177" si="15">"A"&amp;H166</f>
+        <f t="shared" ref="B166:B193" si="15">"A"&amp;H166</f>
         <v>A42</v>
       </c>
       <c r="C166" s="2" t="s">
@@ -6364,24 +6389,28 @@
         <v>4</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D178" s="3">
         <v>23</v>
       </c>
-      <c r="E178" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A45_PP???</v>
-      </c>
-      <c r="F178" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>A45</v>
+      <c r="E178" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H178">
+        <v>45</v>
+      </c>
+      <c r="J178">
+        <v>23</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
@@ -6389,24 +6418,28 @@
         <v>4</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D179" s="3">
         <v>23</v>
       </c>
-      <c r="E179" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A45_PP???</v>
-      </c>
-      <c r="F179" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>A45</v>
+      <c r="E179" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H179">
+        <v>45</v>
+      </c>
+      <c r="J179">
+        <v>23</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
@@ -6414,24 +6447,28 @@
         <v>4</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D180" s="3">
         <v>23</v>
       </c>
-      <c r="E180" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A46_PP???</v>
-      </c>
-      <c r="F180" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>A46</v>
+      <c r="E180" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H180">
+        <v>46</v>
+      </c>
+      <c r="J180">
+        <v>23</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
@@ -6439,324 +6476,376 @@
         <v>4</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D181" s="3">
         <v>23</v>
       </c>
-      <c r="E181" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A46_PP???</v>
-      </c>
-      <c r="F181" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>A46</v>
+      <c r="E181" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="G181" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H181">
+        <v>46</v>
+      </c>
+      <c r="J181">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182" s="3">
+        <v>23</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H182">
+        <v>47</v>
+      </c>
+      <c r="J182">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" s="3">
+        <v>23</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H183">
+        <v>47</v>
+      </c>
+      <c r="J183">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D184" s="3">
+        <v>23</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H184">
+        <v>48</v>
+      </c>
+      <c r="J184">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D185" s="3">
+        <v>23</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H185">
+        <v>48</v>
+      </c>
+      <c r="J185">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D186" s="3">
+        <v>24</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G186" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>4</v>
-      </c>
-      <c r="B182" t="s">
-        <v>20</v>
-      </c>
-      <c r="C182" t="s">
+      <c r="H186">
+        <v>49</v>
+      </c>
+      <c r="J186">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D187" s="3">
+        <v>24</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H187">
+        <v>49</v>
+      </c>
+      <c r="J187">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D188" s="3">
+        <v>24</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H188">
+        <v>50</v>
+      </c>
+      <c r="J188">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189" s="3">
+        <v>24</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F189" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H189">
+        <v>50</v>
+      </c>
+      <c r="J189">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C190" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D182">
-        <v>23</v>
-      </c>
-      <c r="E182" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A47_PP3</v>
-      </c>
-      <c r="F182" t="str">
-        <f t="shared" si="12"/>
-        <v>A47</v>
-      </c>
-      <c r="G182" t="s">
+      <c r="D190" s="3">
+        <v>24</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G190" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>4</v>
-      </c>
-      <c r="B183" t="s">
-        <v>20</v>
-      </c>
-      <c r="C183" t="s">
+      <c r="H190">
+        <v>51</v>
+      </c>
+      <c r="J190">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C191" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D183">
-        <v>23</v>
-      </c>
-      <c r="E183" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A47_PP6</v>
-      </c>
-      <c r="F183" t="str">
-        <f t="shared" si="12"/>
-        <v>A47</v>
-      </c>
-      <c r="G183" t="s">
+      <c r="D191" s="3">
+        <v>24</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G191" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>4</v>
-      </c>
-      <c r="B184" t="s">
-        <v>22</v>
-      </c>
-      <c r="C184" t="s">
+      <c r="H191">
+        <v>51</v>
+      </c>
+      <c r="J191">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C192" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D184">
-        <v>23</v>
-      </c>
-      <c r="E184" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A48_PP4</v>
-      </c>
-      <c r="F184" t="str">
-        <f t="shared" si="12"/>
-        <v>A48</v>
-      </c>
-      <c r="G184" t="s">
+      <c r="D192" s="3">
+        <v>24</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G192" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>4</v>
-      </c>
-      <c r="B185" t="s">
-        <v>22</v>
-      </c>
-      <c r="C185" t="s">
+      <c r="H192">
+        <v>52</v>
+      </c>
+      <c r="J192">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C193" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D185">
-        <v>23</v>
-      </c>
-      <c r="E185" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A48_PP5</v>
-      </c>
-      <c r="F185" t="str">
-        <f t="shared" si="12"/>
-        <v>A48</v>
-      </c>
-      <c r="G185" t="s">
+      <c r="D193" s="3">
+        <v>24</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G193" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>4</v>
-      </c>
-      <c r="B186" t="s">
+      <c r="H193">
+        <v>52</v>
+      </c>
+      <c r="J193">
         <v>24</v>
-      </c>
-      <c r="C186" t="s">
-        <v>5</v>
-      </c>
-      <c r="D186">
-        <v>23</v>
-      </c>
-      <c r="E186" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A49_PP1</v>
-      </c>
-      <c r="F186" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A49</v>
-      </c>
-      <c r="G186" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>4</v>
-      </c>
-      <c r="B187" t="s">
-        <v>24</v>
-      </c>
-      <c r="C187" t="s">
-        <v>12</v>
-      </c>
-      <c r="D187">
-        <v>23</v>
-      </c>
-      <c r="E187" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A49_PP8</v>
-      </c>
-      <c r="F187" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A49</v>
-      </c>
-      <c r="G187" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>4</v>
-      </c>
-      <c r="B188" t="s">
-        <v>25</v>
-      </c>
-      <c r="C188" t="s">
-        <v>6</v>
-      </c>
-      <c r="D188">
-        <v>23</v>
-      </c>
-      <c r="E188" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A50_PP2</v>
-      </c>
-      <c r="F188" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A50</v>
-      </c>
-      <c r="G188" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>4</v>
-      </c>
-      <c r="B189" t="s">
-        <v>25</v>
-      </c>
-      <c r="C189" t="s">
-        <v>11</v>
-      </c>
-      <c r="D189">
-        <v>23</v>
-      </c>
-      <c r="E189" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A50_PP7</v>
-      </c>
-      <c r="F189" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A50</v>
-      </c>
-      <c r="G189" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>4</v>
-      </c>
-      <c r="B190" t="s">
-        <v>26</v>
-      </c>
-      <c r="C190" t="s">
-        <v>7</v>
-      </c>
-      <c r="D190">
-        <v>23</v>
-      </c>
-      <c r="E190" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A51_PP3</v>
-      </c>
-      <c r="F190" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A51</v>
-      </c>
-      <c r="G190" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>4</v>
-      </c>
-      <c r="B191" t="s">
-        <v>26</v>
-      </c>
-      <c r="C191" t="s">
-        <v>10</v>
-      </c>
-      <c r="D191">
-        <v>23</v>
-      </c>
-      <c r="E191" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A51_PP6</v>
-      </c>
-      <c r="F191" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A51</v>
-      </c>
-      <c r="G191" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>4</v>
-      </c>
-      <c r="B192" t="s">
-        <v>27</v>
-      </c>
-      <c r="C192" t="s">
-        <v>8</v>
-      </c>
-      <c r="D192">
-        <v>23</v>
-      </c>
-      <c r="E192" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A52_PP4</v>
-      </c>
-      <c r="F192" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A52</v>
-      </c>
-      <c r="G192" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>4</v>
-      </c>
-      <c r="B193" t="s">
-        <v>27</v>
-      </c>
-      <c r="C193" t="s">
-        <v>9</v>
-      </c>
-      <c r="D193">
-        <v>23</v>
-      </c>
-      <c r="E193" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB023_A52_PP5</v>
-      </c>
-      <c r="F193" s="4" t="str">
-        <f t="shared" si="12"/>
-        <v>A52</v>
-      </c>
-      <c r="G193" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -6769,7 +6858,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J17" sqref="A2:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7333,280 +7422,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
there was problem with pipetting, and plate 25 doesn't have 4 replicates. plate A26 has replicates in 5,6,7,8
</commit_message>
<xml_diff>
--- a/DAB/aliquot_plates/NGS.Plates.Barcodes.DAB2017.Final.xlsx
+++ b/DAB/aliquot_plates/NGS.Plates.Barcodes.DAB2017.Final.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="42">
   <si>
     <t>Aliquot Plate</t>
   </si>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J193"/>
+  <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,11 +2736,11 @@
         <v>9</v>
       </c>
       <c r="E67" s="1" t="str">
-        <f t="shared" ref="E67:E130" si="5">A67&amp;"0"&amp;D67&amp;"_"&amp;B67&amp;"_"&amp;C67</f>
+        <f t="shared" ref="E67:E128" si="5">A67&amp;"0"&amp;D67&amp;"_"&amp;B67&amp;"_"&amp;C67</f>
         <v>DAB09_A17_PP8</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f t="shared" ref="F67:F130" si="6">B67</f>
+        <f t="shared" ref="F67:F128" si="6">B67</f>
         <v>A17</v>
       </c>
       <c r="G67" s="1" t="str">
@@ -3008,7 +3008,7 @@
         <v>A19</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f t="shared" ref="G75:G138" si="9">A75&amp;D75</f>
+        <f t="shared" ref="G75:G136" si="9">A75&amp;D75</f>
         <v>DAB10</v>
       </c>
       <c r="H75">
@@ -3782,8 +3782,8 @@
         <v>4</v>
       </c>
       <c r="B99" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>A25</v>
+        <f>"A"&amp;H99</f>
+        <v>A26</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>12</v>
@@ -3793,18 +3793,18 @@
       </c>
       <c r="E99" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB013_A25_PP8</v>
+        <v>DAB013_A26_PP8</v>
       </c>
       <c r="F99" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A25</v>
+        <v>A26</v>
       </c>
       <c r="G99" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB13</v>
       </c>
       <c r="H99">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J99">
         <v>13</v>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="B101" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>A25</v>
+        <v>A26</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>11</v>
@@ -3859,18 +3859,18 @@
       </c>
       <c r="E101" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB013_A25_PP7</v>
+        <v>DAB013_A26_PP7</v>
       </c>
       <c r="F101" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A25</v>
+        <v>A26</v>
       </c>
       <c r="G101" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB13</v>
       </c>
       <c r="H101">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J101">
         <v>13</v>
@@ -3881,18 +3881,18 @@
         <v>4</v>
       </c>
       <c r="B102" s="2" t="str">
-        <f t="shared" ref="B102:B133" si="10">"A"&amp;H102</f>
+        <f t="shared" ref="B102:B131" si="10">"A"&amp;H102</f>
         <v>A26</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D102" s="2">
         <v>13</v>
       </c>
       <c r="E102" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB013_A26_PP3</v>
+        <v>DAB013_A26_PP6</v>
       </c>
       <c r="F102" s="2" t="str">
         <f t="shared" si="6"/>
@@ -3918,14 +3918,14 @@
         <v>A26</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D103" s="2">
         <v>13</v>
       </c>
       <c r="E103" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB013_A26_PP6</v>
+        <v>DAB013_A26_PP5</v>
       </c>
       <c r="F103" s="2" t="str">
         <f t="shared" si="6"/>
@@ -3948,31 +3948,31 @@
       </c>
       <c r="B104" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A26</v>
+        <v>A27</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D104" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E104" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB013_A26_PP4</v>
+        <v>DAB014_A27_PP1</v>
       </c>
       <c r="F104" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A26</v>
+        <v>A27</v>
       </c>
       <c r="G104" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB13</v>
+        <v>DAB14</v>
       </c>
       <c r="H104">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J104">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
@@ -3981,31 +3981,31 @@
       </c>
       <c r="B105" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A26</v>
+        <v>A27</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D105" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E105" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB013_A26_PP5</v>
+        <v>DAB014_A27_PP8</v>
       </c>
       <c r="F105" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A26</v>
+        <v>A27</v>
       </c>
       <c r="G105" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB13</v>
+        <v>DAB14</v>
       </c>
       <c r="H105">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J105">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
@@ -4017,14 +4017,14 @@
         <v>A27</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D106" s="2">
         <v>14</v>
       </c>
       <c r="E106" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A27_PP1</v>
+        <v>DAB014_A27_PP2</v>
       </c>
       <c r="F106" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4050,14 +4050,14 @@
         <v>A27</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D107" s="2">
         <v>14</v>
       </c>
       <c r="E107" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A27_PP8</v>
+        <v>DAB014_A27_PP7</v>
       </c>
       <c r="F107" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4080,28 +4080,28 @@
       </c>
       <c r="B108" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A27</v>
+        <v>A28</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D108" s="2">
         <v>14</v>
       </c>
       <c r="E108" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A27_PP2</v>
+        <v>DAB014_A28_PP3</v>
       </c>
       <c r="F108" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A27</v>
+        <v>A28</v>
       </c>
       <c r="G108" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB14</v>
       </c>
       <c r="H108">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J108">
         <v>14</v>
@@ -4113,28 +4113,28 @@
       </c>
       <c r="B109" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A27</v>
+        <v>A28</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D109" s="2">
         <v>14</v>
       </c>
       <c r="E109" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A27_PP7</v>
+        <v>DAB014_A28_PP6</v>
       </c>
       <c r="F109" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A27</v>
+        <v>A28</v>
       </c>
       <c r="G109" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB14</v>
       </c>
       <c r="H109">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J109">
         <v>14</v>
@@ -4149,14 +4149,14 @@
         <v>A28</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D110" s="2">
         <v>14</v>
       </c>
       <c r="E110" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A28_PP3</v>
+        <v>DAB014_A28_PP4</v>
       </c>
       <c r="F110" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4182,14 +4182,14 @@
         <v>A28</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D111" s="2">
         <v>14</v>
       </c>
       <c r="E111" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A28_PP6</v>
+        <v>DAB014_A28_PP5</v>
       </c>
       <c r="F111" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4212,31 +4212,31 @@
       </c>
       <c r="B112" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A28</v>
+        <v>A29</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D112" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E112" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A28_PP4</v>
+        <v>DAB015_A29_PP1</v>
       </c>
       <c r="F112" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A28</v>
+        <v>A29</v>
       </c>
       <c r="G112" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB14</v>
+        <v>DAB15</v>
       </c>
       <c r="H112">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J112">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
@@ -4245,31 +4245,31 @@
       </c>
       <c r="B113" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A28</v>
+        <v>A29</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D113" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E113" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB014_A28_PP5</v>
+        <v>DAB015_A29_PP8</v>
       </c>
       <c r="F113" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A28</v>
+        <v>A29</v>
       </c>
       <c r="G113" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB14</v>
+        <v>DAB15</v>
       </c>
       <c r="H113">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J113">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
@@ -4281,14 +4281,14 @@
         <v>A29</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D114" s="2">
         <v>15</v>
       </c>
       <c r="E114" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A29_PP1</v>
+        <v>DAB015_A29_PP2</v>
       </c>
       <c r="F114" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4314,14 +4314,14 @@
         <v>A29</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D115" s="2">
         <v>15</v>
       </c>
       <c r="E115" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A29_PP8</v>
+        <v>DAB015_A29_PP7</v>
       </c>
       <c r="F115" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4344,28 +4344,28 @@
       </c>
       <c r="B116" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A29</v>
+        <v>A30</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D116" s="2">
         <v>15</v>
       </c>
       <c r="E116" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A29_PP2</v>
+        <v>DAB015_A30_PP3</v>
       </c>
       <c r="F116" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A29</v>
+        <v>A30</v>
       </c>
       <c r="G116" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB15</v>
       </c>
       <c r="H116">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J116">
         <v>15</v>
@@ -4377,28 +4377,28 @@
       </c>
       <c r="B117" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A29</v>
+        <v>A30</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D117" s="2">
         <v>15</v>
       </c>
       <c r="E117" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A29_PP7</v>
+        <v>DAB015_A30_PP6</v>
       </c>
       <c r="F117" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A29</v>
+        <v>A30</v>
       </c>
       <c r="G117" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB15</v>
       </c>
       <c r="H117">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J117">
         <v>15</v>
@@ -4413,14 +4413,14 @@
         <v>A30</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D118" s="2">
         <v>15</v>
       </c>
       <c r="E118" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A30_PP3</v>
+        <v>DAB015_A30_PP4</v>
       </c>
       <c r="F118" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4446,14 +4446,14 @@
         <v>A30</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D119" s="2">
         <v>15</v>
       </c>
       <c r="E119" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A30_PP6</v>
+        <v>DAB015_A30_PP5</v>
       </c>
       <c r="F119" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4476,31 +4476,31 @@
       </c>
       <c r="B120" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A30</v>
+        <v>A31</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D120" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E120" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A30_PP4</v>
+        <v>DAB016_A31_PP1</v>
       </c>
       <c r="F120" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A30</v>
+        <v>A31</v>
       </c>
       <c r="G120" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB15</v>
+        <v>DAB16</v>
       </c>
       <c r="H120">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J120">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
@@ -4509,31 +4509,31 @@
       </c>
       <c r="B121" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A30</v>
+        <v>A31</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D121" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E121" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB015_A30_PP5</v>
+        <v>DAB016_A31_PP8</v>
       </c>
       <c r="F121" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A30</v>
+        <v>A31</v>
       </c>
       <c r="G121" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB15</v>
+        <v>DAB16</v>
       </c>
       <c r="H121">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J121">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
@@ -4545,14 +4545,14 @@
         <v>A31</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D122" s="2">
         <v>16</v>
       </c>
       <c r="E122" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB016_A31_PP1</v>
+        <v>DAB016_A31_PP2</v>
       </c>
       <c r="F122" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4578,14 +4578,14 @@
         <v>A31</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D123" s="2">
         <v>16</v>
       </c>
       <c r="E123" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB016_A31_PP8</v>
+        <v>DAB016_A31_PP7</v>
       </c>
       <c r="F123" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4608,28 +4608,28 @@
       </c>
       <c r="B124" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A31</v>
+        <v>A32</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D124" s="2">
         <v>16</v>
       </c>
       <c r="E124" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB016_A31_PP2</v>
+        <v>DAB016_A32_PP3</v>
       </c>
       <c r="F124" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A31</v>
+        <v>A32</v>
       </c>
       <c r="G124" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB16</v>
       </c>
       <c r="H124">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J124">
         <v>16</v>
@@ -4641,28 +4641,28 @@
       </c>
       <c r="B125" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A31</v>
+        <v>A32</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D125" s="2">
         <v>16</v>
       </c>
       <c r="E125" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB016_A31_PP7</v>
+        <v>DAB016_A32_PP6</v>
       </c>
       <c r="F125" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A31</v>
+        <v>A32</v>
       </c>
       <c r="G125" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB16</v>
       </c>
       <c r="H125">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J125">
         <v>16</v>
@@ -4677,14 +4677,14 @@
         <v>A32</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D126" s="2">
         <v>16</v>
       </c>
       <c r="E126" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB016_A32_PP3</v>
+        <v>DAB016_A32_PP4</v>
       </c>
       <c r="F126" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4710,14 +4710,14 @@
         <v>A32</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D127" s="2">
         <v>16</v>
       </c>
       <c r="E127" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB016_A32_PP6</v>
+        <v>DAB016_A32_PP5</v>
       </c>
       <c r="F127" s="2" t="str">
         <f t="shared" si="6"/>
@@ -4740,31 +4740,31 @@
       </c>
       <c r="B128" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A32</v>
+        <v>A33</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D128" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E128" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>DAB016_A32_PP4</v>
+        <v>DAB017_A33_PP1</v>
       </c>
       <c r="F128" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>A32</v>
+        <v>A33</v>
       </c>
       <c r="G128" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB16</v>
+        <v>DAB17</v>
       </c>
       <c r="H128">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J128">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
@@ -4773,31 +4773,31 @@
       </c>
       <c r="B129" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>A32</v>
+        <v>A33</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D129" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E129" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>DAB016_A32_PP5</v>
+        <f t="shared" ref="E129:E175" si="11">A129&amp;"0"&amp;D129&amp;"_"&amp;B129&amp;"_"&amp;C129</f>
+        <v>DAB017_A33_PP8</v>
       </c>
       <c r="F129" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>A32</v>
+        <f t="shared" ref="F129:F175" si="12">B129</f>
+        <v>A33</v>
       </c>
       <c r="G129" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB16</v>
+        <v>DAB17</v>
       </c>
       <c r="H129">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J129">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
@@ -4809,17 +4809,17 @@
         <v>A33</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D130" s="2">
         <v>17</v>
       </c>
       <c r="E130" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>DAB017_A33_PP1</v>
+        <f t="shared" si="11"/>
+        <v>DAB017_A33_PP2</v>
       </c>
       <c r="F130" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>A33</v>
       </c>
       <c r="G130" s="2" t="str">
@@ -4842,17 +4842,17 @@
         <v>A33</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D131" s="2">
         <v>17</v>
       </c>
       <c r="E131" s="2" t="str">
-        <f t="shared" ref="E131:E193" si="11">A131&amp;"0"&amp;D131&amp;"_"&amp;B131&amp;"_"&amp;C131</f>
-        <v>DAB017_A33_PP8</v>
+        <f t="shared" si="11"/>
+        <v>DAB017_A33_PP7</v>
       </c>
       <c r="F131" s="2" t="str">
-        <f t="shared" ref="F131:F193" si="12">B131</f>
+        <f t="shared" si="12"/>
         <v>A33</v>
       </c>
       <c r="G131" s="2" t="str">
@@ -4871,29 +4871,29 @@
         <v>4</v>
       </c>
       <c r="B132" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>A33</v>
+        <f t="shared" ref="B132:B163" si="13">"A"&amp;H132</f>
+        <v>A34</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D132" s="2">
         <v>17</v>
       </c>
       <c r="E132" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB017_A33_PP2</v>
+        <v>DAB017_A34_PP3</v>
       </c>
       <c r="F132" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A33</v>
+        <v>A34</v>
       </c>
       <c r="G132" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB17</v>
       </c>
       <c r="H132">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J132">
         <v>17</v>
@@ -4904,29 +4904,29 @@
         <v>4</v>
       </c>
       <c r="B133" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>A33</v>
+        <f t="shared" si="13"/>
+        <v>A34</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D133" s="2">
         <v>17</v>
       </c>
       <c r="E133" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB017_A33_PP7</v>
+        <v>DAB017_A34_PP6</v>
       </c>
       <c r="F133" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A33</v>
+        <v>A34</v>
       </c>
       <c r="G133" s="2" t="str">
         <f t="shared" si="9"/>
         <v>DAB17</v>
       </c>
       <c r="H133">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J133">
         <v>17</v>
@@ -4937,18 +4937,18 @@
         <v>4</v>
       </c>
       <c r="B134" s="2" t="str">
-        <f t="shared" ref="B134:B165" si="13">"A"&amp;H134</f>
+        <f t="shared" si="13"/>
         <v>A34</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D134" s="2">
         <v>17</v>
       </c>
       <c r="E134" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB017_A34_PP3</v>
+        <v>DAB017_A34_PP4</v>
       </c>
       <c r="F134" s="2" t="str">
         <f t="shared" si="12"/>
@@ -4974,14 +4974,14 @@
         <v>A34</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D135" s="2">
         <v>17</v>
       </c>
       <c r="E135" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB017_A34_PP6</v>
+        <v>DAB017_A34_PP5</v>
       </c>
       <c r="F135" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5004,31 +5004,31 @@
       </c>
       <c r="B136" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A34</v>
+        <v>A35</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D136" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E136" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB017_A34_PP4</v>
+        <v>DAB018_A35_PP1</v>
       </c>
       <c r="F136" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A34</v>
+        <v>A35</v>
       </c>
       <c r="G136" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>DAB17</v>
+        <v>DAB18</v>
       </c>
       <c r="H136">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J136">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
@@ -5037,31 +5037,31 @@
       </c>
       <c r="B137" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A34</v>
+        <v>A35</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D137" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E137" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB017_A34_PP5</v>
+        <v>DAB018_A35_PP8</v>
       </c>
       <c r="F137" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A34</v>
+        <v>A35</v>
       </c>
       <c r="G137" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>DAB17</v>
+        <f t="shared" ref="G137:G175" si="14">A137&amp;D137</f>
+        <v>DAB18</v>
       </c>
       <c r="H137">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J137">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
@@ -5073,21 +5073,21 @@
         <v>A35</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D138" s="2">
         <v>18</v>
       </c>
       <c r="E138" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A35_PP1</v>
+        <v>DAB018_A35_PP2</v>
       </c>
       <c r="F138" s="2" t="str">
         <f t="shared" si="12"/>
         <v>A35</v>
       </c>
       <c r="G138" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>DAB18</v>
       </c>
       <c r="H138">
@@ -5106,21 +5106,21 @@
         <v>A35</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D139" s="2">
         <v>18</v>
       </c>
       <c r="E139" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A35_PP8</v>
+        <v>DAB018_A35_PP7</v>
       </c>
       <c r="F139" s="2" t="str">
         <f t="shared" si="12"/>
         <v>A35</v>
       </c>
       <c r="G139" s="2" t="str">
-        <f t="shared" ref="G139:G193" si="14">A139&amp;D139</f>
+        <f t="shared" si="14"/>
         <v>DAB18</v>
       </c>
       <c r="H139">
@@ -5136,28 +5136,28 @@
       </c>
       <c r="B140" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A35</v>
+        <v>A36</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D140" s="2">
         <v>18</v>
       </c>
       <c r="E140" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A35_PP2</v>
+        <v>DAB018_A36_PP3</v>
       </c>
       <c r="F140" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A35</v>
+        <v>A36</v>
       </c>
       <c r="G140" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB18</v>
       </c>
       <c r="H140">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J140">
         <v>18</v>
@@ -5169,28 +5169,28 @@
       </c>
       <c r="B141" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A35</v>
+        <v>A36</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D141" s="2">
         <v>18</v>
       </c>
       <c r="E141" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A35_PP7</v>
+        <v>DAB018_A36_PP6</v>
       </c>
       <c r="F141" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A35</v>
+        <v>A36</v>
       </c>
       <c r="G141" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB18</v>
       </c>
       <c r="H141">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J141">
         <v>18</v>
@@ -5205,14 +5205,14 @@
         <v>A36</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D142" s="2">
         <v>18</v>
       </c>
       <c r="E142" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A36_PP3</v>
+        <v>DAB018_A36_PP4</v>
       </c>
       <c r="F142" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5238,14 +5238,14 @@
         <v>A36</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D143" s="2">
         <v>18</v>
       </c>
       <c r="E143" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A36_PP6</v>
+        <v>DAB018_A36_PP5</v>
       </c>
       <c r="F143" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5268,31 +5268,31 @@
       </c>
       <c r="B144" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A36</v>
+        <v>A37</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D144" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E144" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A36_PP4</v>
+        <v>DAB019_A37_PP1</v>
       </c>
       <c r="F144" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A36</v>
+        <v>A37</v>
       </c>
       <c r="G144" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB18</v>
+        <v>DAB19</v>
       </c>
       <c r="H144">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J144">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
@@ -5301,31 +5301,31 @@
       </c>
       <c r="B145" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A36</v>
+        <v>A37</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D145" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E145" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB018_A36_PP5</v>
+        <v>DAB019_A37_PP8</v>
       </c>
       <c r="F145" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A36</v>
+        <v>A37</v>
       </c>
       <c r="G145" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB18</v>
+        <v>DAB19</v>
       </c>
       <c r="H145">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J145">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
@@ -5337,14 +5337,14 @@
         <v>A37</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D146" s="2">
         <v>19</v>
       </c>
       <c r="E146" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A37_PP1</v>
+        <v>DAB019_A37_PP2</v>
       </c>
       <c r="F146" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5370,14 +5370,14 @@
         <v>A37</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D147" s="2">
         <v>19</v>
       </c>
       <c r="E147" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A37_PP8</v>
+        <v>DAB019_A37_PP7</v>
       </c>
       <c r="F147" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5400,28 +5400,28 @@
       </c>
       <c r="B148" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A37</v>
+        <v>A38</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D148" s="2">
         <v>19</v>
       </c>
       <c r="E148" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A37_PP2</v>
+        <v>DAB019_A38_PP3</v>
       </c>
       <c r="F148" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A37</v>
+        <v>A38</v>
       </c>
       <c r="G148" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB19</v>
       </c>
       <c r="H148">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J148">
         <v>19</v>
@@ -5433,28 +5433,28 @@
       </c>
       <c r="B149" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A37</v>
+        <v>A38</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D149" s="2">
         <v>19</v>
       </c>
       <c r="E149" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A37_PP7</v>
+        <v>DAB019_A38_PP6</v>
       </c>
       <c r="F149" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A37</v>
+        <v>A38</v>
       </c>
       <c r="G149" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB19</v>
       </c>
       <c r="H149">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J149">
         <v>19</v>
@@ -5469,14 +5469,14 @@
         <v>A38</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D150" s="2">
         <v>19</v>
       </c>
       <c r="E150" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A38_PP3</v>
+        <v>DAB019_A38_PP4</v>
       </c>
       <c r="F150" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5502,14 +5502,14 @@
         <v>A38</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D151" s="2">
         <v>19</v>
       </c>
       <c r="E151" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A38_PP6</v>
+        <v>DAB019_A38_PP5</v>
       </c>
       <c r="F151" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5532,31 +5532,31 @@
       </c>
       <c r="B152" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A38</v>
+        <v>A39</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D152" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E152" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A38_PP4</v>
+        <v>DAB020_A39_PP1</v>
       </c>
       <c r="F152" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A38</v>
+        <v>A39</v>
       </c>
       <c r="G152" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB19</v>
+        <v>DAB20</v>
       </c>
       <c r="H152">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J152">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
@@ -5565,31 +5565,31 @@
       </c>
       <c r="B153" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A38</v>
+        <v>A39</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D153" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E153" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB019_A38_PP5</v>
+        <v>DAB020_A39_PP8</v>
       </c>
       <c r="F153" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A38</v>
+        <v>A39</v>
       </c>
       <c r="G153" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB19</v>
+        <v>DAB20</v>
       </c>
       <c r="H153">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J153">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
@@ -5601,14 +5601,14 @@
         <v>A39</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D154" s="2">
         <v>20</v>
       </c>
       <c r="E154" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A39_PP1</v>
+        <v>DAB020_A39_PP2</v>
       </c>
       <c r="F154" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5634,14 +5634,14 @@
         <v>A39</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D155" s="2">
         <v>20</v>
       </c>
       <c r="E155" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A39_PP8</v>
+        <v>DAB020_A39_PP7</v>
       </c>
       <c r="F155" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5664,28 +5664,28 @@
       </c>
       <c r="B156" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A39</v>
+        <v>A40</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D156" s="2">
         <v>20</v>
       </c>
       <c r="E156" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A39_PP2</v>
+        <v>DAB020_A40_PP3</v>
       </c>
       <c r="F156" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A39</v>
+        <v>A40</v>
       </c>
       <c r="G156" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB20</v>
       </c>
       <c r="H156">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J156">
         <v>20</v>
@@ -5697,28 +5697,28 @@
       </c>
       <c r="B157" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A39</v>
+        <v>A40</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D157" s="2">
         <v>20</v>
       </c>
       <c r="E157" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A39_PP7</v>
+        <v>DAB020_A40_PP6</v>
       </c>
       <c r="F157" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A39</v>
+        <v>A40</v>
       </c>
       <c r="G157" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB20</v>
       </c>
       <c r="H157">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J157">
         <v>20</v>
@@ -5733,14 +5733,14 @@
         <v>A40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D158" s="2">
         <v>20</v>
       </c>
       <c r="E158" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A40_PP3</v>
+        <v>DAB020_A40_PP4</v>
       </c>
       <c r="F158" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5766,14 +5766,14 @@
         <v>A40</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D159" s="2">
         <v>20</v>
       </c>
       <c r="E159" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A40_PP6</v>
+        <v>DAB020_A40_PP5</v>
       </c>
       <c r="F159" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5796,31 +5796,31 @@
       </c>
       <c r="B160" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A40</v>
+        <v>A41</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D160" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E160" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A40_PP4</v>
+        <v>DAB021_A41_PP1</v>
       </c>
       <c r="F160" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A40</v>
+        <v>A41</v>
       </c>
       <c r="G160" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB20</v>
+        <v>DAB21</v>
       </c>
       <c r="H160">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J160">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
@@ -5829,31 +5829,31 @@
       </c>
       <c r="B161" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>A40</v>
+        <v>A41</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D161" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E161" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB020_A40_PP5</v>
+        <v>DAB021_A41_PP8</v>
       </c>
       <c r="F161" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A40</v>
+        <v>A41</v>
       </c>
       <c r="G161" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB20</v>
+        <v>DAB21</v>
       </c>
       <c r="H161">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J161">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
@@ -5865,14 +5865,14 @@
         <v>A41</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D162" s="2">
         <v>21</v>
       </c>
       <c r="E162" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A41_PP1</v>
+        <v>DAB021_A41_PP2</v>
       </c>
       <c r="F162" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5898,14 +5898,14 @@
         <v>A41</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D163" s="2">
         <v>21</v>
       </c>
       <c r="E163" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A41_PP8</v>
+        <v>DAB021_A41_PP7</v>
       </c>
       <c r="F163" s="2" t="str">
         <f t="shared" si="12"/>
@@ -5927,29 +5927,29 @@
         <v>4</v>
       </c>
       <c r="B164" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>A41</v>
+        <f t="shared" ref="B164:B175" si="15">"A"&amp;H164</f>
+        <v>A42</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D164" s="2">
         <v>21</v>
       </c>
       <c r="E164" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A41_PP2</v>
+        <v>DAB021_A42_PP3</v>
       </c>
       <c r="F164" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A41</v>
+        <v>A42</v>
       </c>
       <c r="G164" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB21</v>
       </c>
       <c r="H164">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J164">
         <v>21</v>
@@ -5960,29 +5960,29 @@
         <v>4</v>
       </c>
       <c r="B165" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>A41</v>
+        <f t="shared" si="15"/>
+        <v>A42</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D165" s="2">
         <v>21</v>
       </c>
       <c r="E165" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A41_PP7</v>
+        <v>DAB021_A42_PP6</v>
       </c>
       <c r="F165" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A41</v>
+        <v>A42</v>
       </c>
       <c r="G165" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB21</v>
       </c>
       <c r="H165">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J165">
         <v>21</v>
@@ -5993,18 +5993,18 @@
         <v>4</v>
       </c>
       <c r="B166" s="2" t="str">
-        <f t="shared" ref="B166:B193" si="15">"A"&amp;H166</f>
+        <f t="shared" si="15"/>
         <v>A42</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D166" s="2">
         <v>21</v>
       </c>
       <c r="E166" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A42_PP3</v>
+        <v>DAB021_A42_PP4</v>
       </c>
       <c r="F166" s="2" t="str">
         <f t="shared" si="12"/>
@@ -6030,14 +6030,14 @@
         <v>A42</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D167" s="2">
         <v>21</v>
       </c>
       <c r="E167" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A42_PP6</v>
+        <v>DAB021_A42_PP5</v>
       </c>
       <c r="F167" s="2" t="str">
         <f t="shared" si="12"/>
@@ -6060,31 +6060,31 @@
       </c>
       <c r="B168" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>A42</v>
+        <v>A43</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D168" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E168" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A42_PP4</v>
+        <v>DAB022_A43_PP1</v>
       </c>
       <c r="F168" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A42</v>
+        <v>A43</v>
       </c>
       <c r="G168" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB21</v>
+        <v>DAB22</v>
       </c>
       <c r="H168">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J168">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
@@ -6093,31 +6093,31 @@
       </c>
       <c r="B169" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>A42</v>
+        <v>A43</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D169" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E169" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB021_A42_PP5</v>
+        <v>DAB022_A43_PP8</v>
       </c>
       <c r="F169" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A42</v>
+        <v>A43</v>
       </c>
       <c r="G169" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>DAB21</v>
+        <v>DAB22</v>
       </c>
       <c r="H169">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J169">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
@@ -6129,14 +6129,14 @@
         <v>A43</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D170" s="2">
         <v>22</v>
       </c>
       <c r="E170" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB022_A43_PP1</v>
+        <v>DAB022_A43_PP2</v>
       </c>
       <c r="F170" s="2" t="str">
         <f t="shared" si="12"/>
@@ -6162,14 +6162,14 @@
         <v>A43</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D171" s="2">
         <v>22</v>
       </c>
       <c r="E171" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB022_A43_PP8</v>
+        <v>DAB022_A43_PP7</v>
       </c>
       <c r="F171" s="2" t="str">
         <f t="shared" si="12"/>
@@ -6192,28 +6192,28 @@
       </c>
       <c r="B172" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>A43</v>
+        <v>A44</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D172" s="2">
         <v>22</v>
       </c>
       <c r="E172" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB022_A43_PP2</v>
+        <v>DAB022_A44_PP3</v>
       </c>
       <c r="F172" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A43</v>
+        <v>A44</v>
       </c>
       <c r="G172" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB22</v>
       </c>
       <c r="H172">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J172">
         <v>22</v>
@@ -6225,28 +6225,28 @@
       </c>
       <c r="B173" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>A43</v>
+        <v>A44</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D173" s="2">
         <v>22</v>
       </c>
       <c r="E173" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB022_A43_PP7</v>
+        <v>DAB022_A44_PP6</v>
       </c>
       <c r="F173" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>A43</v>
+        <v>A44</v>
       </c>
       <c r="G173" s="2" t="str">
         <f t="shared" si="14"/>
         <v>DAB22</v>
       </c>
       <c r="H173">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J173">
         <v>22</v>
@@ -6261,14 +6261,14 @@
         <v>A44</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D174" s="2">
         <v>22</v>
       </c>
       <c r="E174" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB022_A44_PP3</v>
+        <v>DAB022_A44_PP4</v>
       </c>
       <c r="F174" s="2" t="str">
         <f t="shared" si="12"/>
@@ -6294,14 +6294,14 @@
         <v>A44</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D175" s="2">
         <v>22</v>
       </c>
       <c r="E175" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>DAB022_A44_PP6</v>
+        <v>DAB022_A44_PP5</v>
       </c>
       <c r="F175" s="2" t="str">
         <f t="shared" si="12"/>
@@ -6319,69 +6319,61 @@
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B176" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>A44</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D176" s="2">
-        <v>22</v>
-      </c>
-      <c r="E176" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB022_A44_PP4</v>
-      </c>
-      <c r="F176" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>A44</v>
-      </c>
-      <c r="G176" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>DAB22</v>
+      <c r="A176" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176" s="3">
+        <v>23</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="H176">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J176">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B177" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>A44</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D177" s="2">
-        <v>22</v>
-      </c>
-      <c r="E177" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>DAB022_A44_PP5</v>
-      </c>
-      <c r="F177" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>A44</v>
-      </c>
-      <c r="G177" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>DAB22</v>
+      <c r="A177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D177" s="3">
+        <v>23</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="H177">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J177">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
@@ -6389,25 +6381,25 @@
         <v>4</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D178" s="3">
         <v>23</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G178" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H178">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J178">
         <v>23</v>
@@ -6418,25 +6410,25 @@
         <v>4</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D179" s="3">
         <v>23</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H179">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J179">
         <v>23</v>
@@ -6447,25 +6439,25 @@
         <v>4</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D180" s="3">
         <v>23</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G180" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H180">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J180">
         <v>23</v>
@@ -6476,25 +6468,25 @@
         <v>4</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D181" s="3">
         <v>23</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G181" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H181">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J181">
         <v>23</v>
@@ -6505,25 +6497,25 @@
         <v>4</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D182" s="3">
         <v>23</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G182" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H182">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J182">
         <v>23</v>
@@ -6534,25 +6526,25 @@
         <v>4</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D183" s="3">
         <v>23</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G183" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H183">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J183">
         <v>23</v>
@@ -6563,28 +6555,28 @@
         <v>4</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D184" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H184">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J184">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
@@ -6592,28 +6584,28 @@
         <v>4</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D185" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H185">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J185">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
@@ -6621,25 +6613,25 @@
         <v>4</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D186" s="3">
         <v>24</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G186" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H186">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J186">
         <v>24</v>
@@ -6650,25 +6642,25 @@
         <v>4</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D187" s="3">
         <v>24</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G187" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H187">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J187">
         <v>24</v>
@@ -6679,25 +6671,25 @@
         <v>4</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D188" s="3">
         <v>24</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G188" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H188">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J188">
         <v>24</v>
@@ -6708,25 +6700,25 @@
         <v>4</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D189" s="3">
         <v>24</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G189" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H189">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J189">
         <v>24</v>
@@ -6737,25 +6729,25 @@
         <v>4</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D190" s="3">
         <v>24</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G190" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H190">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J190">
         <v>24</v>
@@ -6766,85 +6758,27 @@
         <v>4</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D191" s="3">
         <v>24</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G191" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H191">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J191">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D192" s="3">
-        <v>24</v>
-      </c>
-      <c r="E192" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F192" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G192" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H192">
-        <v>52</v>
-      </c>
-      <c r="J192">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D193" s="3">
-        <v>24</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F193" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G193" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H193">
-        <v>52</v>
-      </c>
-      <c r="J193">
         <v>24</v>
       </c>
     </row>

</xml_diff>